<commit_message>
chore: docs and templates update (#4243)
update to fit with catalogue data model >4.x
</commit_message>
<xml_diff>
--- a/docs/resources/Mappings.xlsx
+++ b/docs/resources/Mappings.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA345CF-738B-4FAE-AFE5-2AA9704F68CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE2B27E-7A31-4A64-8120-CDB3372FA93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{B3EFD73E-CA91-47FF-85F1-7718F0622768}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12000" xr2:uid="{F86F0FFA-F849-435E-8F15-A7532F91F404}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dataset mappings" sheetId="2" r:id="rId1"/>
-    <sheet name="Variable mappings" sheetId="1" r:id="rId2"/>
+    <sheet name="Dataset mappings" sheetId="1" r:id="rId1"/>
+    <sheet name="Variable mappings" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,30 +39,39 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
+    <t>syntax</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>target dataset</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>source dataset</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
     <t>comments</t>
   </si>
   <si>
-    <t>syntax</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>match</t>
   </si>
   <si>
+    <t>repeats</t>
+  </si>
+  <si>
     <t>target variable</t>
   </si>
   <si>
-    <t>target dataset</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
     <t>source variables other datasets.name</t>
   </si>
   <si>
@@ -70,15 +79,6 @@
   </si>
   <si>
     <t>source variables</t>
-  </si>
-  <si>
-    <t>source dataset</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>order</t>
   </si>
 </sst>
 </file>
@@ -449,36 +449,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4403B478-48E4-493E-A3ED-B8E9B7AEBC0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567CEEA9-5F71-49AF-BB90-1AD5AB1FBBB8}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -487,54 +496,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B90E19C-96E0-4119-8FBB-05870296906E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58A07B1-53BA-40D4-9576-224AC8829486}">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>